<commit_message>
FVSOnline: Fully rely on databaseDescription.xlsx for table descriptions and datatypes.
git-svn-id: svn+ssh://svn.code.sf.net/p/open-fvs/code/rFVS@2375 90b89b48-9230-0de4-5065-812dd12741b8
</commit_message>
<xml_diff>
--- a/shinyFVSOnline/databaseDescription.xlsx
+++ b/shinyFVSOnline/databaseDescription.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="24"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="OutputTableDescriptions" sheetId="1" state="visible" r:id="rId2"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3156" uniqueCount="1438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3164" uniqueCount="1440">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -327,7 +327,7 @@
     <t xml:space="preserve">Case Identification</t>
   </si>
   <si>
-    <t xml:space="preserve">Character</t>
+    <t xml:space="preserve">Text</t>
   </si>
   <si>
     <t xml:space="preserve">Unique FVS case identifier that corresponds to the FVS_Cases table</t>
@@ -2880,7 +2880,7 @@
     <t xml:space="preserve">dClimMort</t>
   </si>
   <si>
-    <t xml:space="preserve">The probability that a tree will die due to climate change corresponding to the amount of change expected with an elevation change of 300 m. The actual rate may be different for each tree because it is based on the year the tree was born. What is reported here is the basal-area-weighted average rate for trees of a given species. Values reported here reflect multipliers coded using field 2 of the MortMult keyword. Also see the MXDEN MULT information below as it also affects mortality.</t>
+    <t xml:space="preserve">The probability that a tree will die due to climate change corresponding to the amount of change expected with an elevation change of 300 m. The actual rate may be different for each tree because it is based on the year the tree was born. What is reported here is the basal-area-weighted average rate for trees of a given species. Values reported here reflect multipliers coded using field 2 of the MortMult keyword. Also see the MxDenMult information below as it also affects mortality.</t>
   </si>
   <si>
     <t xml:space="preserve">GrowthMult</t>
@@ -3696,6 +3696,15 @@
     <t xml:space="preserve">Stand identification code. Not read by FVS when previously set, but may be used for querying purposes.</t>
   </si>
   <si>
+    <t xml:space="preserve">StandPlot_CN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stand/Plot ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not used by FVSOnline</t>
+  </si>
+  <si>
     <t xml:space="preserve">Variant Identification</t>
   </si>
   <si>
@@ -4252,9 +4261,6 @@
   </si>
   <si>
     <t xml:space="preserve">Not read by FVS when previously set, but may be used for querying purposes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StandPlot_CN</t>
   </si>
   <si>
     <t xml:space="preserve">Plot Control Number</t>
@@ -4459,7 +4465,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4489,12 +4495,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -4552,12 +4552,12 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4594,10 +4594,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4626,18 +4622,18 @@
   </sheetPr>
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="91.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.6"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4645,7 +4641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="34.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -4653,7 +4649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="56.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -4661,7 +4657,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="56.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -4669,7 +4665,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -4677,7 +4673,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="34.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -4685,7 +4681,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="34.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -4693,7 +4689,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="23.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -4701,7 +4697,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="56.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -4709,7 +4705,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="56.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -4717,7 +4713,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="34.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -4725,7 +4721,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="34.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -4733,7 +4729,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -4741,7 +4737,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -4749,7 +4745,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="56.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -4757,7 +4753,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -4765,7 +4761,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -4773,7 +4769,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -4781,7 +4777,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -4789,7 +4785,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="34.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -4797,7 +4793,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="34.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -4805,7 +4801,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>42</v>
       </c>
@@ -4813,7 +4809,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -4821,7 +4817,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>46</v>
       </c>
@@ -4829,7 +4825,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="56.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>48</v>
       </c>
@@ -4837,7 +4833,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -4845,7 +4841,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
@@ -4853,7 +4849,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>54</v>
       </c>
@@ -4861,7 +4857,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="56.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
@@ -4888,7 +4884,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5367,7 +5363,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5846,7 +5842,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6087,7 +6083,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6398,7 +6394,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6570,7 +6566,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6923,7 +6919,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7374,7 +7370,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7741,13 +7737,13 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="27.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="71.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.6"/>
@@ -8066,7 +8062,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8349,7 +8345,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8562,7 +8558,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8872,7 +8868,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9015,7 +9011,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9310,7 +9306,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9562,8 +9558,8 @@
   </sheetPr>
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10083,8 +10079,8 @@
   </sheetPr>
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10210,7 +10206,7 @@
       <c r="A9" s="6" t="s">
         <v>910</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="3" t="s">
         <v>911</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -10308,8 +10304,8 @@
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10620,12 +10616,12 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="6" width="23.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="6" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.6"/>
   </cols>
@@ -10873,7 +10869,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11128,7 +11124,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11932,7 +11928,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12447,7 +12443,7 @@
       <c r="A2" s="6" t="s">
         <v>1177</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>1178</v>
       </c>
     </row>
@@ -12455,7 +12451,7 @@
       <c r="A3" s="6" t="s">
         <v>1179</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>1178</v>
       </c>
     </row>
@@ -12483,16 +12479,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="19.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="38.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.6"/>
@@ -12513,941 +12509,969 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>1183</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>1184</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>1185</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>1187</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>1186</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B6" s="9" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>1187</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>1189</v>
-      </c>
-      <c r="C5" s="10" t="s">
+      <c r="D6" s="9" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>1190</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+      <c r="D7" s="9" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>1191</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
-        <v>1192</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>1193</v>
-      </c>
-      <c r="C7" s="10" t="s">
+      <c r="D8" s="9" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>1194</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
-        <v>1195</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>1196</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="D9" s="9" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="9" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>1197</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
-        <v>1198</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>1199</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D9" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>1200</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+    <row r="11" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="9" t="s">
         <v>1201</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>1202</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="10" t="s">
+      <c r="C11" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>1203</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
+    <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9" t="s">
         <v>1204</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>1205</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C12" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
-        <v>1207</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>1208</v>
-      </c>
-      <c r="C12" s="10" t="s">
+      <c r="D13" s="9" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="9" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>1209</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
-        <v>1210</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>1211</v>
-      </c>
-      <c r="C13" s="10" t="s">
+      <c r="D14" s="9" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="9" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>1212</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
-        <v>1213</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="D15" s="9" t="s">
+        <v>1215</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="9" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>1215</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
-        <v>1216</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>1217</v>
-      </c>
-      <c r="C15" s="10" t="s">
+      <c r="D16" s="9" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="9" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>1218</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
-        <v>1219</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>1219</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="D17" s="9" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="9" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>1220</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
-        <v>1221</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>1222</v>
-      </c>
-      <c r="C17" s="10" t="s">
+      <c r="D18" s="9" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="9" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>1223</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="s">
-        <v>1224</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>1225</v>
-      </c>
-      <c r="C18" s="10" t="s">
+      <c r="D19" s="9" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>1226</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
+      <c r="D20" s="9" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>1227</v>
-      </c>
-      <c r="C19" s="10" t="s">
+      <c r="B21" s="9" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>1228</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
-        <v>1229</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>1230</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="10" t="s">
+      <c r="D21" s="9" t="s">
         <v>1231</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="9" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="9" t="s">
         <v>587</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>1232</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>1233</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="s">
-        <v>1234</v>
-      </c>
-      <c r="B22" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>1235</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="10" t="s">
+      <c r="C23" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>1236</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
+    <row r="24" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9" t="s">
         <v>1237</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>1238</v>
       </c>
-      <c r="C23" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="10" t="s">
+      <c r="C24" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>1239</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="s">
+    <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="9" t="s">
         <v>1240</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>1241</v>
       </c>
-      <c r="C24" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="10" t="s">
+      <c r="C25" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>1242</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10" t="s">
+    <row r="26" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="9" t="s">
         <v>1243</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>1244</v>
       </c>
-      <c r="C25" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="10" t="s">
+      <c r="C26" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>1245</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="10" t="s">
+    <row r="27" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="9" t="s">
         <v>1246</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>1247</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="10" t="s">
+      <c r="C27" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="9" t="s">
         <v>1248</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="10" t="s">
+    <row r="28" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="9" t="s">
         <v>1249</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>1250</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C28" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="9" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D27" s="10" t="s">
-        <v>1251</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="10" t="s">
-        <v>1252</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>1253</v>
-      </c>
-      <c r="C28" s="10" t="s">
+      <c r="D29" s="9" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="10" t="s">
-        <v>1254</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="s">
-        <v>1255</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>1256</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="10" t="s">
+      <c r="D30" s="9" t="s">
         <v>1257</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10" t="s">
+    <row r="31" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="9" t="s">
         <v>1258</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>1259</v>
       </c>
-      <c r="C30" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="10" t="s">
+      <c r="C31" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>1260</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10" t="s">
+    <row r="32" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="9" t="s">
         <v>1261</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>1262</v>
       </c>
-      <c r="C31" s="10" t="s">
+      <c r="C32" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="9" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D31" s="10" t="s">
-        <v>1263</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="10" t="s">
-        <v>1264</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>1265</v>
-      </c>
-      <c r="C32" s="10" t="s">
+      <c r="D33" s="9" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="9" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D32" s="10" t="s">
-        <v>1266</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10" t="s">
-        <v>1267</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>1268</v>
-      </c>
-      <c r="C33" s="10" t="s">
+      <c r="D34" s="9" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="9" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>1269</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10" t="s">
-        <v>1270</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>1271</v>
-      </c>
-      <c r="C34" s="10" t="s">
+      <c r="D35" s="9" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="9" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D34" s="10" t="s">
-        <v>1272</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10" t="s">
-        <v>1273</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>1274</v>
-      </c>
-      <c r="C35" s="10" t="s">
+      <c r="D36" s="9" t="s">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="9" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C37" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="10" t="s">
-        <v>1275</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10" t="s">
-        <v>1276</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>1277</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D36" s="10" t="s">
+      <c r="D37" s="9" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10" t="s">
+    <row r="38" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="9" t="s">
         <v>1279</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B38" s="9" t="s">
         <v>1280</v>
       </c>
-      <c r="C37" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>1280</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10" t="s">
+      <c r="C38" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="9" t="s">
         <v>1281</v>
       </c>
-      <c r="B38" s="10" t="s">
+    </row>
+    <row r="39" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="9" t="s">
         <v>1282</v>
       </c>
-      <c r="C38" s="10" t="s">
+      <c r="B39" s="9" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>1283</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="9" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C40" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D38" s="10" t="s">
-        <v>1283</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10" t="s">
-        <v>1284</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>1285</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="10" t="s">
+      <c r="D40" s="9" t="s">
         <v>1286</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10" t="s">
+    <row r="41" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="9" t="s">
         <v>1287</v>
       </c>
-      <c r="B40" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>1288</v>
       </c>
-      <c r="C40" s="10" t="s">
+      <c r="C41" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="9" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C42" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D40" s="10" t="s">
-        <v>1289</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10" t="s">
-        <v>1290</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>1291</v>
-      </c>
-      <c r="C41" s="10" t="s">
+      <c r="D42" s="9" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="9" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D41" s="10" t="s">
-        <v>1292</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="10" t="s">
-        <v>1293</v>
-      </c>
-      <c r="B42" s="10" t="s">
+      <c r="D43" s="9" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="9" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B44" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="C42" s="10" t="s">
+      <c r="C44" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D42" s="10" t="s">
-        <v>1294</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="10" t="s">
-        <v>1295</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>1295</v>
-      </c>
-      <c r="C43" s="10" t="s">
+      <c r="D44" s="9" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="9" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D43" s="10" t="s">
-        <v>1296</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="10" t="s">
-        <v>1297</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>1297</v>
-      </c>
-      <c r="C44" s="10" t="s">
+      <c r="D45" s="9" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="9" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D44" s="10" t="s">
-        <v>1298</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="10" t="s">
-        <v>1299</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>1300</v>
-      </c>
-      <c r="C45" s="10" t="s">
+      <c r="D46" s="9" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="105" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="9" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D45" s="10" t="s">
-        <v>1301</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="10" t="s">
-        <v>1302</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>1303</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D46" s="10" t="s">
+      <c r="D47" s="9" t="s">
         <v>1304</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="10" t="s">
+    <row r="48" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="9" t="s">
         <v>1305</v>
       </c>
-      <c r="B47" s="10" t="s">
+      <c r="B48" s="9" t="s">
         <v>1306</v>
       </c>
-      <c r="C47" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D47" s="10" t="s">
+      <c r="C48" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D48" s="9" t="s">
         <v>1307</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="10" t="s">
+    <row r="49" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="9" t="s">
         <v>1308</v>
       </c>
-      <c r="B48" s="10" t="s">
+      <c r="B49" s="9" t="s">
         <v>1309</v>
       </c>
-      <c r="C48" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D48" s="10" t="s">
+      <c r="C49" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D49" s="9" t="s">
         <v>1310</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="10" t="s">
+    <row r="50" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="9" t="s">
         <v>1311</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="B50" s="9" t="s">
         <v>1312</v>
       </c>
-      <c r="C49" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D49" s="10" t="s">
+      <c r="C50" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D50" s="9" t="s">
         <v>1313</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="10" t="s">
+    <row r="51" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="9" t="s">
         <v>1314</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B51" s="9" t="s">
         <v>1315</v>
       </c>
-      <c r="C50" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D50" s="10" t="s">
+      <c r="C51" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51" s="9" t="s">
         <v>1316</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="10" t="s">
+    <row r="52" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="9" t="s">
         <v>1317</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B52" s="9" t="s">
         <v>1318</v>
       </c>
-      <c r="C51" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D51" s="10" t="s">
+      <c r="C52" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D52" s="9" t="s">
         <v>1319</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="10" t="s">
+    <row r="53" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="9" t="s">
         <v>1320</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="B53" s="9" t="s">
         <v>1321</v>
       </c>
-      <c r="C52" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D52" s="10" t="s">
+      <c r="C53" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D53" s="9" t="s">
         <v>1322</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="10" t="s">
+    <row r="54" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="9" t="s">
         <v>1323</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="B54" s="9" t="s">
         <v>1324</v>
       </c>
-      <c r="C53" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D53" s="10" t="s">
+      <c r="C54" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D54" s="9" t="s">
         <v>1325</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="10" t="s">
+    <row r="55" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="9" t="s">
         <v>1326</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B55" s="9" t="s">
         <v>1327</v>
       </c>
-      <c r="C54" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D54" s="10" t="s">
+      <c r="C55" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D55" s="9" t="s">
         <v>1328</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="10" t="s">
+    <row r="56" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="9" t="s">
         <v>1329</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B56" s="9" t="s">
         <v>1330</v>
       </c>
-      <c r="C55" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D55" s="10" t="s">
+      <c r="C56" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D56" s="9" t="s">
         <v>1331</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="10" t="s">
+    <row r="57" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="9" t="s">
         <v>1332</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="B57" s="9" t="s">
         <v>1333</v>
       </c>
-      <c r="C56" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D56" s="10" t="s">
+      <c r="C57" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D57" s="9" t="s">
         <v>1334</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="10" t="s">
+    <row r="58" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="9" t="s">
         <v>1335</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B58" s="9" t="s">
         <v>1336</v>
       </c>
-      <c r="C57" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D57" s="10" t="s">
+      <c r="C58" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D58" s="9" t="s">
         <v>1337</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="10" t="s">
+    <row r="59" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="9" t="s">
         <v>1338</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B59" s="9" t="s">
         <v>1339</v>
       </c>
-      <c r="C58" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D58" s="10" t="s">
+      <c r="C59" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D59" s="9" t="s">
         <v>1340</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="10" t="s">
+    <row r="60" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="9" t="s">
         <v>1341</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B60" s="9" t="s">
         <v>1342</v>
       </c>
-      <c r="C59" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D59" s="10" t="s">
+      <c r="C60" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D60" s="9" t="s">
         <v>1343</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="10" t="s">
+    <row r="61" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="9" t="s">
         <v>1344</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B61" s="9" t="s">
         <v>1345</v>
       </c>
-      <c r="C60" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D60" s="10" t="s">
+      <c r="C61" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D61" s="9" t="s">
         <v>1346</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="10" t="s">
+    <row r="62" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="9" t="s">
         <v>1347</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="B62" s="9" t="s">
         <v>1348</v>
       </c>
-      <c r="C61" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D61" s="10" t="s">
+      <c r="C62" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D62" s="9" t="s">
         <v>1349</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="10" t="s">
+    <row r="63" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="9" t="s">
         <v>1350</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B63" s="9" t="s">
         <v>1351</v>
       </c>
-      <c r="C62" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D62" s="10" t="s">
+      <c r="C63" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D63" s="9" t="s">
         <v>1352</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="10" t="s">
+    <row r="64" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="9" t="s">
         <v>1353</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B64" s="9" t="s">
         <v>1354</v>
       </c>
-      <c r="C63" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D63" s="10" t="s">
+      <c r="C64" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D64" s="9" t="s">
         <v>1355</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="10" t="s">
+    <row r="65" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="9" t="s">
         <v>1356</v>
       </c>
-      <c r="B64" s="10" t="s">
+      <c r="B65" s="9" t="s">
         <v>1357</v>
       </c>
-      <c r="C64" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D64" s="10" t="s">
+      <c r="C65" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D65" s="9" t="s">
         <v>1358</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="10" t="s">
+    <row r="66" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="9" t="s">
         <v>1359</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B66" s="9" t="s">
         <v>1360</v>
       </c>
-      <c r="C65" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D65" s="10" t="s">
+      <c r="C66" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D66" s="9" t="s">
         <v>1361</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="10" t="s">
+    <row r="67" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="9" t="s">
         <v>1362</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B67" s="9" t="s">
         <v>1363</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C67" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>1364</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="9" t="s">
+        <v>1365</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C68" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D66" s="10" t="s">
-        <v>1364</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="10" t="s">
-        <v>1365</v>
-      </c>
-      <c r="B67" s="10" t="s">
-        <v>1366</v>
-      </c>
-      <c r="C67" s="10" t="s">
+      <c r="D68" s="9" t="s">
+        <v>1367</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="9" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D67" s="10" t="s">
-        <v>1367</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="10" t="s">
-        <v>1368</v>
-      </c>
-      <c r="B68" s="10" t="s">
-        <v>1369</v>
-      </c>
-      <c r="C68" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D68" s="10" t="s">
+      <c r="D69" s="9" t="s">
         <v>1370</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="9" t="s">
+        <v>1371</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>1372</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>1373</v>
       </c>
     </row>
   </sheetData>
@@ -13468,8 +13492,8 @@
   </sheetPr>
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13494,981 +13518,981 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>1371</v>
+      <c r="D2" s="9" t="s">
+        <v>1374</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>1184</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>1371</v>
+      <c r="D3" s="9" t="s">
+        <v>1374</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
-        <v>1372</v>
+      <c r="A4" s="9" t="s">
+        <v>1186</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>1373</v>
+        <v>1375</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>1374</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
-        <v>1375</v>
+      <c r="A5" s="9" t="s">
+        <v>1377</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>1376</v>
+        <v>1378</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>1377</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
-        <v>1378</v>
+      <c r="A6" s="9" t="s">
+        <v>1380</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>1379</v>
+        <v>1381</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>1380</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>1186</v>
-      </c>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="9" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>1187</v>
+      <c r="D7" s="9" t="s">
+        <v>1190</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>1189</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="A8" s="9" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>1190</v>
+      <c r="D8" s="9" t="s">
+        <v>1193</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="90" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>1191</v>
+      <c r="D9" s="9" t="s">
+        <v>1194</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
-        <v>1192</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>1193</v>
-      </c>
-      <c r="C10" s="10" t="s">
+      <c r="A10" s="9" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>1194</v>
+      <c r="D10" s="9" t="s">
+        <v>1197</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
-        <v>1195</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>1196</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="A11" s="9" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>1199</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>1197</v>
+      <c r="D11" s="9" t="s">
+        <v>1200</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
-        <v>1198</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>1199</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>1200</v>
+      <c r="A12" s="9" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>1202</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>1203</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
-        <v>1201</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>1202</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>1203</v>
+      <c r="A13" s="9" t="s">
+        <v>1204</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>1205</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>1206</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
-        <v>1204</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>1205</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="A14" s="9" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>1208</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>1206</v>
+      <c r="D14" s="9" t="s">
+        <v>1209</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
-        <v>1207</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>1208</v>
-      </c>
-      <c r="C15" s="10" t="s">
+      <c r="A15" s="9" t="s">
+        <v>1210</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>1211</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>1209</v>
+      <c r="D15" s="9" t="s">
+        <v>1212</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
-        <v>1210</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>1211</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="A16" s="9" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>1212</v>
+      <c r="D16" s="9" t="s">
+        <v>1215</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
-        <v>1213</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>1214</v>
-      </c>
-      <c r="C17" s="10" t="s">
+      <c r="A17" s="9" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>1217</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>1215</v>
+      <c r="D17" s="9" t="s">
+        <v>1218</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="s">
-        <v>1216</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>1217</v>
-      </c>
-      <c r="C18" s="10" t="s">
+      <c r="A18" s="9" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>1218</v>
+      <c r="D18" s="9" t="s">
+        <v>1221</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
-        <v>1219</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>1219</v>
-      </c>
-      <c r="C19" s="10" t="s">
+      <c r="A19" s="9" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>1222</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>1220</v>
+      <c r="D19" s="9" t="s">
+        <v>1223</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
-        <v>1221</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>1222</v>
-      </c>
-      <c r="C20" s="10" t="s">
+      <c r="A20" s="9" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="10" t="s">
-        <v>1223</v>
+      <c r="D20" s="9" t="s">
+        <v>1226</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
-        <v>1224</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>1225</v>
-      </c>
-      <c r="C21" s="10" t="s">
+      <c r="A21" s="9" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>1226</v>
+      <c r="D21" s="9" t="s">
+        <v>1229</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>1227</v>
-      </c>
-      <c r="C22" s="10" t="s">
+      <c r="B22" s="9" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D22" s="10" t="s">
-        <v>1228</v>
+      <c r="D22" s="9" t="s">
+        <v>1231</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
-        <v>1229</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>1230</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>1231</v>
+      <c r="A23" s="9" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>1233</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>1234</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="9" t="s">
         <v>587</v>
       </c>
-      <c r="B24" s="10" t="s">
-        <v>1232</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>1233</v>
+      <c r="B24" s="9" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>1236</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10" t="s">
-        <v>1234</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>1235</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>1236</v>
+      <c r="A25" s="9" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>1239</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="10" t="s">
-        <v>1237</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>1238</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>1239</v>
+      <c r="A26" s="9" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>1241</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>1242</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="10" t="s">
-        <v>1240</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>1241</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>1242</v>
+      <c r="A27" s="9" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>1245</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="10" t="s">
-        <v>1243</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>1244</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>1245</v>
+      <c r="A28" s="9" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>1247</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>1248</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="s">
-        <v>1246</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>1247</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>1248</v>
+      <c r="A29" s="9" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>1251</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10" t="s">
-        <v>1249</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>1250</v>
-      </c>
-      <c r="C30" s="10" t="s">
+      <c r="A30" s="9" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D30" s="10" t="s">
-        <v>1251</v>
+      <c r="D30" s="9" t="s">
+        <v>1254</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10" t="s">
-        <v>1252</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>1253</v>
-      </c>
-      <c r="C31" s="10" t="s">
+      <c r="A31" s="9" t="s">
+        <v>1255</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D31" s="10" t="s">
-        <v>1254</v>
+      <c r="D31" s="9" t="s">
+        <v>1257</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="10" t="s">
-        <v>1255</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>1256</v>
-      </c>
-      <c r="C32" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>1257</v>
+      <c r="A32" s="9" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>1260</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10" t="s">
-        <v>1258</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>1259</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>1260</v>
+      <c r="A33" s="9" t="s">
+        <v>1261</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>1263</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10" t="s">
-        <v>1261</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>1262</v>
-      </c>
-      <c r="C34" s="10" t="s">
+      <c r="A34" s="9" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C34" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D34" s="10" t="s">
-        <v>1263</v>
+      <c r="D34" s="9" t="s">
+        <v>1266</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10" t="s">
-        <v>1264</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>1265</v>
-      </c>
-      <c r="C35" s="10" t="s">
+      <c r="A35" s="9" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D35" s="10" t="s">
-        <v>1266</v>
+      <c r="D35" s="9" t="s">
+        <v>1269</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10" t="s">
-        <v>1267</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>1268</v>
-      </c>
-      <c r="C36" s="10" t="s">
+      <c r="A36" s="9" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D36" s="10" t="s">
-        <v>1269</v>
+      <c r="D36" s="9" t="s">
+        <v>1272</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10" t="s">
-        <v>1270</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>1271</v>
-      </c>
-      <c r="C37" s="10" t="s">
+      <c r="A37" s="9" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>1274</v>
+      </c>
+      <c r="C37" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D37" s="10" t="s">
-        <v>1272</v>
+      <c r="D37" s="9" t="s">
+        <v>1275</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10" t="s">
-        <v>1273</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>1274</v>
-      </c>
-      <c r="C38" s="10" t="s">
+      <c r="A38" s="9" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>1277</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D38" s="10" t="s">
-        <v>1275</v>
+      <c r="D38" s="9" t="s">
+        <v>1278</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10" t="s">
-        <v>1276</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>1277</v>
-      </c>
-      <c r="C39" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>1278</v>
+      <c r="A39" s="9" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>1280</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>1281</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="10" t="s">
-        <v>1279</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>1280</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>1280</v>
+      <c r="A40" s="9" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>1283</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="10" t="s">
-        <v>1281</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>1282</v>
-      </c>
-      <c r="C41" s="10" t="s">
+      <c r="A41" s="9" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D41" s="10" t="s">
-        <v>1283</v>
+      <c r="D41" s="9" t="s">
+        <v>1286</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="10" t="s">
-        <v>1284</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>1285</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>1286</v>
+      <c r="A42" s="9" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>1289</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="10" t="s">
-        <v>1287</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>1288</v>
-      </c>
-      <c r="C43" s="10" t="s">
+      <c r="A43" s="9" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C43" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D43" s="10" t="s">
-        <v>1289</v>
+      <c r="D43" s="9" t="s">
+        <v>1292</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="10" t="s">
-        <v>1290</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>1291</v>
-      </c>
-      <c r="C44" s="10" t="s">
+      <c r="A44" s="9" t="s">
+        <v>1293</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C44" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D44" s="10" t="s">
-        <v>1292</v>
+      <c r="D44" s="9" t="s">
+        <v>1295</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="10" t="s">
-        <v>1293</v>
-      </c>
-      <c r="B45" s="10" t="s">
+      <c r="A45" s="9" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B45" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="C45" s="10" t="s">
+      <c r="C45" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D45" s="10" t="s">
-        <v>1294</v>
+      <c r="D45" s="9" t="s">
+        <v>1297</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="10" t="s">
-        <v>1295</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>1295</v>
-      </c>
-      <c r="C46" s="10" t="s">
+      <c r="A46" s="9" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>1298</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D46" s="10" t="s">
-        <v>1296</v>
+      <c r="D46" s="9" t="s">
+        <v>1299</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="10" t="s">
-        <v>1297</v>
-      </c>
-      <c r="B47" s="10" t="s">
-        <v>1297</v>
-      </c>
-      <c r="C47" s="10" t="s">
+      <c r="A47" s="9" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D47" s="10" t="s">
-        <v>1298</v>
+      <c r="D47" s="9" t="s">
+        <v>1301</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="10" t="s">
-        <v>1299</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>1300</v>
-      </c>
-      <c r="C48" s="10" t="s">
+      <c r="A48" s="9" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C48" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D48" s="10" t="s">
-        <v>1301</v>
+      <c r="D48" s="9" t="s">
+        <v>1304</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="10" t="s">
-        <v>1302</v>
-      </c>
-      <c r="B49" s="10" t="s">
-        <v>1303</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>1304</v>
+      <c r="A49" s="9" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>1306</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>1307</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="10" t="s">
-        <v>1305</v>
-      </c>
-      <c r="B50" s="10" t="s">
-        <v>1306</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>1307</v>
+      <c r="A50" s="9" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>1310</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="10" t="s">
-        <v>1308</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>1309</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>1310</v>
+      <c r="A51" s="9" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>1312</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>1313</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="10" t="s">
-        <v>1311</v>
-      </c>
-      <c r="B52" s="10" t="s">
-        <v>1312</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>1313</v>
+      <c r="A52" s="9" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>1315</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>1316</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="10" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B53" s="10" t="s">
-        <v>1315</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>1316</v>
+      <c r="A53" s="9" t="s">
+        <v>1317</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>1318</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>1319</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="10" t="s">
-        <v>1317</v>
-      </c>
-      <c r="B54" s="10" t="s">
-        <v>1318</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>1319</v>
+      <c r="A54" s="9" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>1322</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="10" t="s">
-        <v>1320</v>
-      </c>
-      <c r="B55" s="10" t="s">
-        <v>1321</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D55" s="10" t="s">
-        <v>1322</v>
+      <c r="A55" s="9" t="s">
+        <v>1323</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>1324</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>1325</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="10" t="s">
-        <v>1323</v>
-      </c>
-      <c r="B56" s="10" t="s">
-        <v>1324</v>
-      </c>
-      <c r="C56" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D56" s="10" t="s">
-        <v>1325</v>
+      <c r="A56" s="9" t="s">
+        <v>1326</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>1327</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>1328</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="10" t="s">
-        <v>1326</v>
-      </c>
-      <c r="B57" s="10" t="s">
-        <v>1327</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D57" s="10" t="s">
-        <v>1328</v>
+      <c r="A57" s="9" t="s">
+        <v>1329</v>
+      </c>
+      <c r="B57" s="9" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>1331</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="10" t="s">
-        <v>1329</v>
-      </c>
-      <c r="B58" s="10" t="s">
-        <v>1330</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>1331</v>
+      <c r="A58" s="9" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B58" s="9" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C58" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>1334</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="10" t="s">
-        <v>1332</v>
-      </c>
-      <c r="B59" s="10" t="s">
-        <v>1333</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D59" s="10" t="s">
-        <v>1334</v>
+      <c r="A59" s="9" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C59" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>1337</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="10" t="s">
-        <v>1335</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>1336</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>1337</v>
+      <c r="A60" s="9" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>1340</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="10" t="s">
-        <v>1338</v>
-      </c>
-      <c r="B61" s="10" t="s">
-        <v>1339</v>
-      </c>
-      <c r="C61" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D61" s="10" t="s">
-        <v>1340</v>
+      <c r="A61" s="9" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B61" s="9" t="s">
+        <v>1342</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>1343</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="10" t="s">
-        <v>1341</v>
-      </c>
-      <c r="B62" s="10" t="s">
-        <v>1342</v>
-      </c>
-      <c r="C62" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D62" s="10" t="s">
-        <v>1343</v>
+      <c r="A62" s="9" t="s">
+        <v>1344</v>
+      </c>
+      <c r="B62" s="9" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C62" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>1346</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="10" t="s">
-        <v>1344</v>
-      </c>
-      <c r="B63" s="10" t="s">
-        <v>1345</v>
-      </c>
-      <c r="C63" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>1346</v>
+      <c r="A63" s="9" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B63" s="9" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>1349</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="10" t="s">
-        <v>1347</v>
-      </c>
-      <c r="B64" s="10" t="s">
-        <v>1348</v>
-      </c>
-      <c r="C64" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>1349</v>
+      <c r="A64" s="9" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B64" s="9" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>1352</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="10" t="s">
-        <v>1350</v>
-      </c>
-      <c r="B65" s="10" t="s">
-        <v>1351</v>
-      </c>
-      <c r="C65" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D65" s="10" t="s">
-        <v>1352</v>
+      <c r="A65" s="9" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B65" s="9" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>1355</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="10" t="s">
-        <v>1353</v>
-      </c>
-      <c r="B66" s="10" t="s">
-        <v>1354</v>
-      </c>
-      <c r="C66" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D66" s="10" t="s">
-        <v>1355</v>
+      <c r="A66" s="9" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B66" s="9" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C66" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>1358</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="10" t="s">
-        <v>1356</v>
-      </c>
-      <c r="B67" s="10" t="s">
-        <v>1357</v>
-      </c>
-      <c r="C67" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D67" s="10" t="s">
-        <v>1358</v>
+      <c r="A67" s="9" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>1361</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="10" t="s">
-        <v>1359</v>
-      </c>
-      <c r="B68" s="10" t="s">
-        <v>1360</v>
-      </c>
-      <c r="C68" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D68" s="10" t="s">
-        <v>1361</v>
+      <c r="A68" s="9" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>1363</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>1364</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="10" t="s">
-        <v>1362</v>
-      </c>
-      <c r="B69" s="10" t="s">
-        <v>1363</v>
-      </c>
-      <c r="C69" s="10" t="s">
+      <c r="A69" s="9" t="s">
+        <v>1365</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>1366</v>
+      </c>
+      <c r="C69" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D69" s="10" t="s">
-        <v>1364</v>
+      <c r="D69" s="9" t="s">
+        <v>1367</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="10" t="s">
-        <v>1365</v>
-      </c>
-      <c r="B70" s="10" t="s">
-        <v>1366</v>
-      </c>
-      <c r="C70" s="10" t="s">
+      <c r="A70" s="9" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B70" s="9" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C70" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D70" s="10" t="s">
-        <v>1367</v>
+      <c r="D70" s="9" t="s">
+        <v>1370</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="10" t="s">
-        <v>1369</v>
-      </c>
-      <c r="B71" s="10" t="s">
-        <v>1369</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D71" s="10" t="s">
-        <v>1370</v>
+      <c r="A71" s="9" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B71" s="9" t="s">
+        <v>1372</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>1373</v>
       </c>
     </row>
   </sheetData>
@@ -14489,8 +14513,8 @@
   </sheetPr>
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C31" activeCellId="0" sqref="C31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14517,7 +14541,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>65</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -14526,12 +14550,12 @@
       <c r="C2" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>1371</v>
+      <c r="D2" s="9" t="s">
+        <v>1374</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>1184</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -14540,55 +14564,55 @@
       <c r="C3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>1371</v>
+      <c r="D3" s="9" t="s">
+        <v>1374</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
-        <v>1372</v>
+      <c r="A4" s="10" t="s">
+        <v>1186</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>1373</v>
+        <v>1375</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>1374</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>1378</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>1376</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>1380</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
-        <v>1375</v>
+      <c r="A6" s="10" t="s">
+        <v>1377</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>1379</v>
+        <v>1381</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>1381</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
-        <v>1382</v>
+      <c r="A7" s="10" t="s">
+        <v>1384</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>283</v>
@@ -14597,39 +14621,39 @@
         <v>82</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>1383</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
-        <v>1384</v>
+      <c r="A8" s="10" t="s">
+        <v>1386</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>1385</v>
+        <v>1387</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>1386</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="120" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11" t="s">
-        <v>1387</v>
+      <c r="A9" s="10" t="s">
+        <v>1389</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>1388</v>
+        <v>1390</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>1389</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>288</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -14639,25 +14663,25 @@
         <v>63</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>1390</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="135" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>303</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>1391</v>
+        <v>1393</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>1392</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>306</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -14667,26 +14691,26 @@
         <v>82</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>1393</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="10" t="s">
         <v>309</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>1394</v>
+        <v>1396</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>1395</v>
+        <v>1397</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11" t="s">
-        <v>1396</v>
+      <c r="A14" s="10" t="s">
+        <v>1398</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>313</v>
@@ -14695,231 +14719,231 @@
         <v>82</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>1397</v>
+        <v>1399</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
-        <v>1398</v>
+      <c r="A15" s="10" t="s">
+        <v>1400</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>1399</v>
+        <v>1401</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>1400</v>
+        <v>1402</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="11" t="s">
-        <v>1401</v>
+      <c r="A16" s="10" t="s">
+        <v>1403</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>1402</v>
+        <v>1404</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>1403</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="11" t="s">
-        <v>1404</v>
+      <c r="A17" s="10" t="s">
+        <v>1406</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>1405</v>
+        <v>1407</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>1406</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
-        <v>1407</v>
+      <c r="A18" s="10" t="s">
+        <v>1409</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>1408</v>
+        <v>1410</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>1409</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="11" t="s">
-        <v>1410</v>
+      <c r="A19" s="10" t="s">
+        <v>1412</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>1411</v>
+        <v>1413</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>1412</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="11" t="s">
-        <v>1413</v>
+      <c r="A20" s="10" t="s">
+        <v>1415</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>1416</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>1417</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="10" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>1419</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>1414</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>1415</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="11" t="s">
-        <v>1416</v>
-      </c>
-      <c r="B21" s="6" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="10" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="6" t="s">
         <v>1417</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>1412</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="s">
-        <v>1418</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>1419</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>1415</v>
-      </c>
     </row>
     <row r="23" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="10" t="s">
         <v>290</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>1420</v>
+        <v>1422</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>1421</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="11" t="s">
-        <v>1422</v>
+      <c r="A24" s="10" t="s">
+        <v>1424</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>1423</v>
+        <v>1425</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>1424</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="10" t="s">
         <v>99</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>1425</v>
+        <v>1427</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>1426</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="10" t="s">
         <v>587</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>1427</v>
+        <v>1429</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>97</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>1428</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11" t="s">
-        <v>1229</v>
+      <c r="A27" s="10" t="s">
+        <v>1232</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>1429</v>
+        <v>1431</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>97</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>1430</v>
+        <v>1432</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11" t="s">
-        <v>1221</v>
+      <c r="A28" s="10" t="s">
+        <v>1224</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>1222</v>
+        <v>1225</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>63</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>1431</v>
+        <v>1433</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11" t="s">
-        <v>1432</v>
+      <c r="A29" s="10" t="s">
+        <v>1434</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>1433</v>
+        <v>1435</v>
       </c>
       <c r="C29" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>1434</v>
+        <v>1436</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11" t="s">
-        <v>1435</v>
+      <c r="A30" s="10" t="s">
+        <v>1437</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>1436</v>
+        <v>1438</v>
       </c>
       <c r="C30" s="6" t="s">
         <v>82</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>1437</v>
+        <v>1439</v>
       </c>
     </row>
   </sheetData>
@@ -14940,8 +14964,8 @@
   </sheetPr>
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15392,7 +15416,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15520,8 +15544,8 @@
   </sheetPr>
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15832,7 +15856,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16031,7 +16055,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16272,13 +16296,13 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="80.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="8.57"/>

</xml_diff>

<commit_message>
merge of shinyFVSOnline with shinyFVSOnlineDev for 20200228 release.
git-svn-id: svn+ssh://svn.code.sf.net/p/open-fvs/code/rFVS@2982 90b89b48-9230-0de4-5065-812dd12741b8
</commit_message>
<xml_diff>
--- a/shinyFVSOnline/databaseDescription.xlsx
+++ b/shinyFVSOnline/databaseDescription.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FVS\Project_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michaelashettles\Documents\Program of Work\POW 17\Online FVS\fvssetup\Fvsbin\FVSProjects\Project_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55A794D-396F-4682-A019-D71BA02C5866}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D473678-B052-4EC8-A86E-B6056907ECAF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" firstSheet="25" activeTab="31" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" firstSheet="21" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OutputTableDescriptions" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4448" uniqueCount="1848">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4448" uniqueCount="1851">
   <si>
     <t>Table</t>
   </si>
@@ -5577,42 +5577,6 @@
     <t>Average large-tree diameter growth, or small-tree height growth, scale factors for a species within a given stand. Applied before calibration, these multipliers are used to permanently change the model to a different mean response level.</t>
   </si>
   <si>
-    <t>Hard snags in size class 1 (default=0.0-12.0")</t>
-  </si>
-  <si>
-    <t>Soft snags in size class 1 (default=0.0-12.0")</t>
-  </si>
-  <si>
-    <t>Hard snags in size class 2 (default=12.0-18.0")</t>
-  </si>
-  <si>
-    <t>Hard snags in size class 3 (default=18.0-24.0")</t>
-  </si>
-  <si>
-    <t>Hard snags in size class 4 (default=24.0-30.0")</t>
-  </si>
-  <si>
-    <t>Hard snags in size class 5 (default=30.0-36.0")</t>
-  </si>
-  <si>
-    <t>Hard snags in size class 6 (default=36.0"+)</t>
-  </si>
-  <si>
-    <t>Soft snags in size class 2 (default=12.0-18.0")</t>
-  </si>
-  <si>
-    <t>Soft snags in size class 3 (default=18.0-24.0")</t>
-  </si>
-  <si>
-    <t>Soft snags in size class 4 (default=24.0-30.0")</t>
-  </si>
-  <si>
-    <t>Soft snags in size class 5 (default=30.0-36.0")</t>
-  </si>
-  <si>
-    <t>Soft snags in size class 6 (default=36.0"+)</t>
-  </si>
-  <si>
     <t>FVS_Potfire_East</t>
   </si>
   <si>
@@ -5707,6 +5671,51 @@
   </si>
   <si>
     <t>Basal area per acre (sq ft/acre)</t>
+  </si>
+  <si>
+    <t>Hard snags in size class 1 (default &gt;=0.0")</t>
+  </si>
+  <si>
+    <t>Hard snags in size class 2 (default &gt;=12.0")</t>
+  </si>
+  <si>
+    <t>Hard snags in size class 3 (default &gt;=18.0")</t>
+  </si>
+  <si>
+    <t>Hard snags in size class 4 (default &gt;=24.0")</t>
+  </si>
+  <si>
+    <t>Hard snags in size class 5 (default &gt;=30.0")</t>
+  </si>
+  <si>
+    <t>Hard snags in size class 6 (default &gt;=36.0")</t>
+  </si>
+  <si>
+    <t>Hard snags total (all &gt;=0”)</t>
+  </si>
+  <si>
+    <t>Soft snags in size class 1 (default &gt;=0.0")</t>
+  </si>
+  <si>
+    <t>Soft snags in size class 2 (default &gt;=12.0")</t>
+  </si>
+  <si>
+    <t>Soft snags in size class 3 (default &gt;=18.0")</t>
+  </si>
+  <si>
+    <t>Soft snags in size class 4 (default &gt;=24.0")</t>
+  </si>
+  <si>
+    <t>Soft snags in size class 5 (default &gt;=30.0")</t>
+  </si>
+  <si>
+    <t>Soft snags in size class 6 (default &gt;=36.0")</t>
+  </si>
+  <si>
+    <t>Soft snags total (all &gt;=0”)</t>
+  </si>
+  <si>
+    <t>Hard and soft snags total (all &gt;=0”)</t>
   </si>
 </sst>
 </file>
@@ -6273,7 +6282,7 @@
     </row>
     <row r="20" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>1816</v>
+        <v>1804</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>1667</v>
@@ -8993,7 +9002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>78</v>
       </c>
@@ -9046,7 +9055,7 @@
         <v>99</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>1817</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9060,7 +9069,7 @@
         <v>99</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>1818</v>
+        <v>1806</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9074,7 +9083,7 @@
         <v>99</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>1819</v>
+        <v>1807</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9088,7 +9097,7 @@
         <v>99</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>1820</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -9102,7 +9111,7 @@
         <v>99</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>1821</v>
+        <v>1809</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -9116,7 +9125,7 @@
         <v>99</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>1822</v>
+        <v>1810</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -9130,7 +9139,7 @@
         <v>99</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>1823</v>
+        <v>1811</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9144,7 +9153,7 @@
         <v>99</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>1824</v>
+        <v>1812</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9158,7 +9167,7 @@
         <v>99</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>1825</v>
+        <v>1813</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -9172,7 +9181,7 @@
         <v>99</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>1826</v>
+        <v>1814</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -9186,7 +9195,7 @@
         <v>99</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>1827</v>
+        <v>1815</v>
       </c>
     </row>
   </sheetData>
@@ -9581,7 +9590,7 @@
         <v>99</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>1828</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -9595,7 +9604,7 @@
         <v>99</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>1829</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -9609,7 +9618,7 @@
         <v>99</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>1830</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -9623,7 +9632,7 @@
         <v>99</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>1831</v>
+        <v>1819</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9637,7 +9646,7 @@
         <v>99</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>1832</v>
+        <v>1820</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9651,7 +9660,7 @@
         <v>99</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>1833</v>
+        <v>1821</v>
       </c>
     </row>
   </sheetData>
@@ -12376,8 +12385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:AMK19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12456,7 +12465,7 @@
         <v>99</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>1804</v>
+        <v>1836</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -12470,7 +12479,7 @@
         <v>99</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>1806</v>
+        <v>1837</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -12484,7 +12493,7 @@
         <v>99</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>1807</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -12498,7 +12507,7 @@
         <v>99</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>1808</v>
+        <v>1839</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -12512,7 +12521,7 @@
         <v>99</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>1809</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -12526,7 +12535,7 @@
         <v>99</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>1810</v>
+        <v>1841</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -12540,7 +12549,7 @@
         <v>99</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>764</v>
+        <v>1842</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -12554,7 +12563,7 @@
         <v>99</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>1805</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -12568,7 +12577,7 @@
         <v>99</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>1811</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -12582,7 +12591,7 @@
         <v>99</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>1812</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -12596,7 +12605,7 @@
         <v>99</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>1813</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -12610,7 +12619,7 @@
         <v>99</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>1814</v>
+        <v>1847</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -12624,7 +12633,7 @@
         <v>99</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>1815</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -12638,7 +12647,7 @@
         <v>99</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>778</v>
+        <v>1849</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -12652,12 +12661,12 @@
         <v>99</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>780</v>
+        <v>1850</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13533,7 +13542,7 @@
         <v>99</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>1847</v>
+        <v>1835</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -13575,7 +13584,7 @@
         <v>99</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>1846</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -13589,7 +13598,7 @@
         <v>99</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>1845</v>
+        <v>1833</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -13603,7 +13612,7 @@
         <v>99</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>1844</v>
+        <v>1832</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -13617,7 +13626,7 @@
         <v>99</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>1843</v>
+        <v>1831</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -13631,7 +13640,7 @@
         <v>99</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>1842</v>
+        <v>1830</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -13645,7 +13654,7 @@
         <v>99</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>1841</v>
+        <v>1829</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -13659,7 +13668,7 @@
         <v>99</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>1840</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -13673,7 +13682,7 @@
         <v>99</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>1839</v>
+        <v>1827</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -13687,7 +13696,7 @@
         <v>99</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>1838</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -13701,7 +13710,7 @@
         <v>99</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>1837</v>
+        <v>1825</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>1538</v>
@@ -13746,7 +13755,7 @@
         <v>99</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>1834</v>
+        <v>1822</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -13760,7 +13769,7 @@
         <v>99</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>1835</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -13774,7 +13783,7 @@
         <v>114</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>1836</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -14252,7 +14261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:AMK20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
@@ -16537,7 +16546,7 @@
         <v>99</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>1846</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -16705,7 +16714,7 @@
         <v>114</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>1836</v>
+        <v>1824</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>